<commit_message>
feat: random sampling code
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:U501"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,10 +433,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>330</v>
       </c>
       <c r="C2" t="n">
-        <v>11</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3">
@@ -444,10 +444,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>63</v>
+        <v>449</v>
       </c>
       <c r="C3" t="n">
-        <v>74</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4">
@@ -455,10 +455,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>96</v>
+        <v>238</v>
       </c>
       <c r="C4" t="n">
-        <v>70</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5">
@@ -466,7 +466,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>16</v>
+        <v>436</v>
+      </c>
+      <c r="C5" t="n">
+        <v>426</v>
       </c>
     </row>
     <row r="6">
@@ -474,10 +477,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>90</v>
+        <v>222</v>
       </c>
       <c r="C6" t="n">
-        <v>73</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7">
@@ -485,10 +488,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>86</v>
+        <v>221</v>
       </c>
       <c r="C7" t="n">
-        <v>24</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8">
@@ -496,10 +499,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>54</v>
+        <v>257</v>
       </c>
       <c r="C8" t="n">
-        <v>45</v>
+        <v>78</v>
+      </c>
+      <c r="D8" t="n">
+        <v>411</v>
+      </c>
+      <c r="E8" t="n">
+        <v>454</v>
+      </c>
+      <c r="F8" t="n">
+        <v>254</v>
+      </c>
+      <c r="G8" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="9">
@@ -507,10 +522,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>85</v>
+        <v>262</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>156</v>
+      </c>
+      <c r="D9" t="n">
+        <v>126</v>
+      </c>
+      <c r="E9" t="n">
+        <v>110</v>
+      </c>
+      <c r="F9" t="n">
+        <v>355</v>
       </c>
     </row>
     <row r="10">
@@ -518,16 +542,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>50</v>
+        <v>325</v>
       </c>
       <c r="C10" t="n">
-        <v>14</v>
+        <v>302</v>
       </c>
       <c r="D10" t="n">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>96</v>
+      </c>
+      <c r="F10" t="n">
+        <v>371</v>
+      </c>
+      <c r="G10" t="n">
+        <v>264</v>
       </c>
     </row>
     <row r="11">
@@ -535,7 +565,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>42</v>
+        <v>337</v>
+      </c>
+      <c r="C11" t="n">
+        <v>398</v>
       </c>
     </row>
     <row r="12">
@@ -543,10 +576,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C12" t="n">
-        <v>71</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13">
@@ -554,7 +587,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="C13" t="n">
+        <v>86</v>
       </c>
     </row>
     <row r="14">
@@ -565,7 +601,7 @@
         <v>29</v>
       </c>
       <c r="C14" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15">
@@ -573,10 +609,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="C15" t="n">
-        <v>52</v>
+        <v>265</v>
+      </c>
+      <c r="D15" t="n">
+        <v>135</v>
+      </c>
+      <c r="E15" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="16">
@@ -584,10 +626,64 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="C16" t="n">
-        <v>61</v>
+        <v>290</v>
+      </c>
+      <c r="D16" t="n">
+        <v>121</v>
+      </c>
+      <c r="E16" t="n">
+        <v>147</v>
+      </c>
+      <c r="F16" t="n">
+        <v>74</v>
+      </c>
+      <c r="G16" t="n">
+        <v>440</v>
+      </c>
+      <c r="H16" t="n">
+        <v>260</v>
+      </c>
+      <c r="I16" t="n">
+        <v>109</v>
+      </c>
+      <c r="J16" t="n">
+        <v>481</v>
+      </c>
+      <c r="K16" t="n">
+        <v>457</v>
+      </c>
+      <c r="L16" t="n">
+        <v>266</v>
+      </c>
+      <c r="M16" t="n">
+        <v>12</v>
+      </c>
+      <c r="N16" t="n">
+        <v>101</v>
+      </c>
+      <c r="O16" t="n">
+        <v>190</v>
+      </c>
+      <c r="P16" t="n">
+        <v>271</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>8</v>
+      </c>
+      <c r="R16" t="n">
+        <v>311</v>
+      </c>
+      <c r="S16" t="n">
+        <v>123</v>
+      </c>
+      <c r="T16" t="n">
+        <v>216</v>
+      </c>
+      <c r="U16" t="n">
+        <v>358</v>
       </c>
     </row>
     <row r="17">
@@ -597,13 +693,19 @@
       <c r="B17" t="n">
         <v>92</v>
       </c>
+      <c r="C17" t="n">
+        <v>128</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>49</v>
+        <v>468</v>
+      </c>
+      <c r="C18" t="n">
+        <v>467</v>
       </c>
     </row>
     <row r="19">
@@ -611,22 +713,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>51</v>
+        <v>248</v>
       </c>
       <c r="C19" t="n">
-        <v>7</v>
-      </c>
-      <c r="D19" t="n">
-        <v>44</v>
-      </c>
-      <c r="E19" t="n">
-        <v>40</v>
-      </c>
-      <c r="F19" t="n">
-        <v>37</v>
-      </c>
-      <c r="G19" t="n">
-        <v>79</v>
+        <v>414</v>
       </c>
     </row>
     <row r="20">
@@ -634,7 +724,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>47</v>
+        <v>82</v>
+      </c>
+      <c r="C20" t="n">
+        <v>482</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +735,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>65</v>
+        <v>410</v>
+      </c>
+      <c r="C21" t="n">
+        <v>69</v>
+      </c>
+      <c r="D21" t="n">
+        <v>233</v>
       </c>
     </row>
     <row r="22">
@@ -650,19 +749,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>19</v>
+        <v>348</v>
       </c>
       <c r="C22" t="n">
-        <v>9</v>
+        <v>336</v>
       </c>
       <c r="D22" t="n">
-        <v>20</v>
-      </c>
-      <c r="E22" t="n">
-        <v>91</v>
-      </c>
-      <c r="F22" t="n">
-        <v>33</v>
+        <v>339</v>
       </c>
     </row>
     <row r="23">
@@ -670,7 +763,49 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>12</v>
+        <v>94</v>
+      </c>
+      <c r="C23" t="n">
+        <v>17</v>
+      </c>
+      <c r="D23" t="n">
+        <v>81</v>
+      </c>
+      <c r="E23" t="n">
+        <v>166</v>
+      </c>
+      <c r="F23" t="n">
+        <v>430</v>
+      </c>
+      <c r="G23" t="n">
+        <v>22</v>
+      </c>
+      <c r="H23" t="n">
+        <v>223</v>
+      </c>
+      <c r="I23" t="n">
+        <v>280</v>
+      </c>
+      <c r="J23" t="n">
+        <v>142</v>
+      </c>
+      <c r="K23" t="n">
+        <v>44</v>
+      </c>
+      <c r="L23" t="n">
+        <v>108</v>
+      </c>
+      <c r="M23" t="n">
+        <v>333</v>
+      </c>
+      <c r="N23" t="n">
+        <v>413</v>
+      </c>
+      <c r="O23" t="n">
+        <v>72</v>
+      </c>
+      <c r="P23" t="n">
+        <v>182</v>
       </c>
     </row>
     <row r="24">
@@ -678,10 +813,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>55</v>
+        <v>183</v>
       </c>
       <c r="C24" t="n">
-        <v>46</v>
+        <v>497</v>
       </c>
     </row>
     <row r="25">
@@ -689,10 +824,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C25" t="n">
-        <v>81</v>
+        <v>150</v>
+      </c>
+      <c r="D25" t="n">
+        <v>273</v>
       </c>
     </row>
     <row r="26">
@@ -700,10 +838,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="C26" t="n">
-        <v>32</v>
+        <v>455</v>
       </c>
     </row>
     <row r="27">
@@ -711,10 +849,37 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>10</v>
+        <v>474</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>66</v>
+      </c>
+      <c r="D27" t="n">
+        <v>293</v>
+      </c>
+      <c r="E27" t="n">
+        <v>169</v>
+      </c>
+      <c r="F27" t="n">
+        <v>212</v>
+      </c>
+      <c r="G27" t="n">
+        <v>6</v>
+      </c>
+      <c r="H27" t="n">
+        <v>456</v>
+      </c>
+      <c r="I27" t="n">
+        <v>188</v>
+      </c>
+      <c r="J27" t="n">
+        <v>261</v>
+      </c>
+      <c r="K27" t="n">
+        <v>186</v>
+      </c>
+      <c r="L27" t="n">
+        <v>173</v>
       </c>
     </row>
     <row r="28">
@@ -722,10 +887,49 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C28" t="n">
-        <v>67</v>
+        <v>170</v>
+      </c>
+      <c r="D28" t="n">
+        <v>229</v>
+      </c>
+      <c r="E28" t="n">
+        <v>352</v>
+      </c>
+      <c r="F28" t="n">
+        <v>434</v>
+      </c>
+      <c r="G28" t="n">
+        <v>244</v>
+      </c>
+      <c r="H28" t="n">
+        <v>438</v>
+      </c>
+      <c r="I28" t="n">
+        <v>373</v>
+      </c>
+      <c r="J28" t="n">
+        <v>21</v>
+      </c>
+      <c r="K28" t="n">
+        <v>272</v>
+      </c>
+      <c r="L28" t="n">
+        <v>341</v>
+      </c>
+      <c r="M28" t="n">
+        <v>486</v>
+      </c>
+      <c r="N28" t="n">
+        <v>408</v>
+      </c>
+      <c r="O28" t="n">
+        <v>328</v>
+      </c>
+      <c r="P28" t="n">
+        <v>491</v>
       </c>
     </row>
     <row r="29">
@@ -733,10 +937,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C29" t="n">
-        <v>8</v>
+        <v>460</v>
+      </c>
+      <c r="D29" t="n">
+        <v>100</v>
+      </c>
+      <c r="E29" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="30">
@@ -744,10 +954,34 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>87</v>
+        <v>306</v>
       </c>
       <c r="C30" t="n">
-        <v>18</v>
+        <v>296</v>
+      </c>
+      <c r="D30" t="n">
+        <v>270</v>
+      </c>
+      <c r="E30" t="n">
+        <v>378</v>
+      </c>
+      <c r="F30" t="n">
+        <v>4</v>
+      </c>
+      <c r="G30" t="n">
+        <v>435</v>
+      </c>
+      <c r="H30" t="n">
+        <v>245</v>
+      </c>
+      <c r="I30" t="n">
+        <v>51</v>
+      </c>
+      <c r="J30" t="n">
+        <v>443</v>
+      </c>
+      <c r="K30" t="n">
+        <v>479</v>
       </c>
     </row>
     <row r="31">
@@ -755,10 +989,25 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>83</v>
+        <v>493</v>
       </c>
       <c r="C31" t="n">
-        <v>78</v>
+        <v>472</v>
+      </c>
+      <c r="D31" t="n">
+        <v>80</v>
+      </c>
+      <c r="E31" t="n">
+        <v>207</v>
+      </c>
+      <c r="F31" t="n">
+        <v>117</v>
+      </c>
+      <c r="G31" t="n">
+        <v>217</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -766,10 +1015,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="C32" t="n">
-        <v>25</v>
+        <v>146</v>
+      </c>
+      <c r="D32" t="n">
+        <v>54</v>
+      </c>
+      <c r="E32" t="n">
+        <v>393</v>
       </c>
     </row>
     <row r="33">
@@ -777,10 +1032,25 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>66</v>
+        <v>368</v>
       </c>
       <c r="C33" t="n">
-        <v>75</v>
+        <v>227</v>
+      </c>
+      <c r="D33" t="n">
+        <v>218</v>
+      </c>
+      <c r="E33" t="n">
+        <v>274</v>
+      </c>
+      <c r="F33" t="n">
+        <v>189</v>
+      </c>
+      <c r="G33" t="n">
+        <v>151</v>
+      </c>
+      <c r="H33" t="n">
+        <v>213</v>
       </c>
     </row>
     <row r="34">
@@ -788,10 +1058,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>15</v>
+        <v>394</v>
       </c>
       <c r="C34" t="n">
-        <v>34</v>
+        <v>388</v>
       </c>
     </row>
     <row r="35">
@@ -799,13 +1069,22 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="C35" t="n">
-        <v>88</v>
+        <v>228</v>
       </c>
       <c r="D35" t="n">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="E35" t="n">
+        <v>20</v>
+      </c>
+      <c r="F35" t="n">
+        <v>342</v>
+      </c>
+      <c r="G35" t="n">
+        <v>319</v>
       </c>
     </row>
     <row r="36">
@@ -813,10 +1092,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>53</v>
+        <v>492</v>
       </c>
       <c r="C36" t="n">
-        <v>26</v>
+        <v>415</v>
+      </c>
+      <c r="D36" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="37">
@@ -824,10 +1106,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>22</v>
+        <v>215</v>
       </c>
       <c r="C37" t="n">
-        <v>93</v>
+        <v>180</v>
+      </c>
+      <c r="D37" t="n">
+        <v>285</v>
       </c>
     </row>
     <row r="38">
@@ -835,10 +1120,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>36</v>
+        <v>329</v>
       </c>
       <c r="C38" t="n">
-        <v>21</v>
+        <v>194</v>
+      </c>
+      <c r="D38" t="n">
+        <v>313</v>
+      </c>
+      <c r="E38" t="n">
+        <v>310</v>
+      </c>
+      <c r="F38" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="39">
@@ -846,7 +1140,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>72</v>
+        <v>432</v>
+      </c>
+      <c r="C39" t="n">
+        <v>153</v>
       </c>
     </row>
     <row r="40">
@@ -854,7 +1151,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>17</v>
+        <v>209</v>
+      </c>
+      <c r="C40" t="n">
+        <v>263</v>
       </c>
     </row>
     <row r="41">
@@ -862,7 +1162,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>28</v>
+        <v>157</v>
+      </c>
+      <c r="C41" t="n">
+        <v>152</v>
       </c>
     </row>
     <row r="42">
@@ -870,10 +1173,25 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C42" t="n">
-        <v>89</v>
+        <v>498</v>
+      </c>
+      <c r="D42" t="n">
+        <v>148</v>
+      </c>
+      <c r="E42" t="n">
+        <v>43</v>
+      </c>
+      <c r="F42" t="n">
+        <v>241</v>
+      </c>
+      <c r="G42" t="n">
+        <v>249</v>
+      </c>
+      <c r="H42" t="n">
+        <v>258</v>
       </c>
     </row>
     <row r="43">
@@ -881,10 +1199,22 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>48</v>
+        <v>452</v>
       </c>
       <c r="C43" t="n">
-        <v>38</v>
+        <v>323</v>
+      </c>
+      <c r="D43" t="n">
+        <v>281</v>
+      </c>
+      <c r="E43" t="n">
+        <v>284</v>
+      </c>
+      <c r="F43" t="n">
+        <v>288</v>
+      </c>
+      <c r="G43" t="n">
+        <v>487</v>
       </c>
     </row>
     <row r="44">
@@ -892,10 +1222,25 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>94</v>
+        <v>412</v>
       </c>
       <c r="C44" t="n">
-        <v>23</v>
+        <v>404</v>
+      </c>
+      <c r="D44" t="n">
+        <v>143</v>
+      </c>
+      <c r="E44" t="n">
+        <v>76</v>
+      </c>
+      <c r="F44" t="n">
+        <v>15</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1</v>
+      </c>
+      <c r="H44" t="n">
+        <v>403</v>
       </c>
     </row>
     <row r="45">
@@ -903,7 +1248,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>62</v>
+        <v>428</v>
+      </c>
+      <c r="C45" t="n">
+        <v>423</v>
       </c>
     </row>
     <row r="46">
@@ -911,7 +1259,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>35</v>
+        <v>219</v>
+      </c>
+      <c r="C46" t="n">
+        <v>134</v>
       </c>
     </row>
     <row r="47">
@@ -919,10 +1270,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>57</v>
+        <v>256</v>
       </c>
       <c r="C47" t="n">
-        <v>2</v>
+        <v>484</v>
+      </c>
+      <c r="D47" t="n">
+        <v>422</v>
       </c>
     </row>
     <row r="48">
@@ -930,7 +1284,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>76</v>
+        <v>201</v>
+      </c>
+      <c r="C48" t="n">
+        <v>450</v>
       </c>
     </row>
     <row r="49">
@@ -938,7 +1295,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>69</v>
+        <v>77</v>
+      </c>
+      <c r="C49" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="50">
@@ -946,7 +1306,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>6</v>
+        <v>136</v>
+      </c>
+      <c r="C50" t="n">
+        <v>391</v>
       </c>
     </row>
     <row r="51">
@@ -954,10 +1317,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="C51" t="n">
-        <v>30</v>
+        <v>471</v>
+      </c>
+      <c r="D51" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="52">
@@ -965,10 +1331,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C52" t="n">
-        <v>4</v>
+        <v>416</v>
       </c>
     </row>
     <row r="53">
@@ -976,232 +1342,3090 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>68</v>
+        <v>366</v>
+      </c>
+      <c r="C53" t="n">
+        <v>308</v>
+      </c>
+      <c r="D53" t="n">
+        <v>295</v>
+      </c>
+      <c r="E53" t="n">
+        <v>384</v>
+      </c>
+      <c r="F53" t="n">
+        <v>376</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
         <v>53</v>
       </c>
+      <c r="B54" t="n">
+        <v>324</v>
+      </c>
+      <c r="C54" t="n">
+        <v>381</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
         <v>54</v>
       </c>
+      <c r="B55" t="n">
+        <v>370</v>
+      </c>
+      <c r="C55" t="n">
+        <v>350</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
         <v>55</v>
       </c>
+      <c r="B56" t="n">
+        <v>178</v>
+      </c>
+      <c r="C56" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
         <v>56</v>
       </c>
+      <c r="B57" t="n">
+        <v>320</v>
+      </c>
+      <c r="C57" t="n">
+        <v>496</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
         <v>57</v>
       </c>
+      <c r="B58" t="n">
+        <v>420</v>
+      </c>
+      <c r="C58" t="n">
+        <v>137</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
         <v>58</v>
       </c>
+      <c r="B59" t="n">
+        <v>316</v>
+      </c>
+      <c r="C59" t="n">
+        <v>419</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
         <v>59</v>
       </c>
+      <c r="B60" t="n">
+        <v>47</v>
+      </c>
+      <c r="C60" t="n">
+        <v>344</v>
+      </c>
+      <c r="D60" t="n">
+        <v>162</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
         <v>60</v>
       </c>
+      <c r="B61" t="n">
+        <v>483</v>
+      </c>
+      <c r="C61" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
         <v>61</v>
       </c>
+      <c r="B62" t="n">
+        <v>106</v>
+      </c>
+      <c r="C62" t="n">
+        <v>357</v>
+      </c>
+      <c r="D62" t="n">
+        <v>99</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
         <v>62</v>
       </c>
+      <c r="B63" t="n">
+        <v>65</v>
+      </c>
+      <c r="C63" t="n">
+        <v>447</v>
+      </c>
+      <c r="D63" t="n">
+        <v>463</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
         <v>63</v>
       </c>
+      <c r="B64" t="n">
+        <v>301</v>
+      </c>
+      <c r="C64" t="n">
+        <v>417</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
         <v>64</v>
       </c>
+      <c r="B65" t="n">
+        <v>164</v>
+      </c>
+      <c r="C65" t="n">
+        <v>327</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
         <v>65</v>
       </c>
+      <c r="B66" t="n">
+        <v>446</v>
+      </c>
+      <c r="C66" t="n">
+        <v>210</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
         <v>66</v>
       </c>
+      <c r="B67" t="n">
+        <v>84</v>
+      </c>
+      <c r="C67" t="n">
+        <v>105</v>
+      </c>
+      <c r="D67" t="n">
+        <v>490</v>
+      </c>
+      <c r="E67" t="n">
+        <v>314</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
         <v>67</v>
       </c>
+      <c r="B68" t="n">
+        <v>88</v>
+      </c>
+      <c r="C68" t="n">
+        <v>489</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
         <v>68</v>
       </c>
+      <c r="B69" t="n">
+        <v>469</v>
+      </c>
+      <c r="C69" t="n">
+        <v>480</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
         <v>69</v>
       </c>
+      <c r="B70" t="n">
+        <v>279</v>
+      </c>
+      <c r="C70" t="n">
+        <v>181</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
         <v>70</v>
       </c>
+      <c r="B71" t="n">
+        <v>297</v>
+      </c>
+      <c r="C71" t="n">
+        <v>298</v>
+      </c>
+      <c r="D71" t="n">
+        <v>360</v>
+      </c>
+      <c r="E71" t="n">
+        <v>304</v>
+      </c>
+      <c r="F71" t="n">
+        <v>168</v>
+      </c>
+      <c r="G71" t="n">
+        <v>103</v>
+      </c>
+      <c r="H71" t="n">
+        <v>107</v>
+      </c>
+      <c r="I71" t="n">
+        <v>114</v>
+      </c>
+      <c r="J71" t="n">
+        <v>377</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
         <v>71</v>
       </c>
+      <c r="B72" t="n">
+        <v>289</v>
+      </c>
+      <c r="C72" t="n">
+        <v>441</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
         <v>72</v>
       </c>
+      <c r="B73" t="n">
+        <v>451</v>
+      </c>
+      <c r="C73" t="n">
+        <v>141</v>
+      </c>
+      <c r="D73" t="n">
+        <v>62</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
         <v>73</v>
       </c>
+      <c r="B74" t="n">
+        <v>478</v>
+      </c>
+      <c r="C74" t="n">
+        <v>122</v>
+      </c>
+      <c r="D74" t="n">
+        <v>448</v>
+      </c>
+      <c r="E74" t="n">
+        <v>202</v>
+      </c>
+      <c r="F74" t="n">
+        <v>386</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
         <v>74</v>
       </c>
+      <c r="B75" t="n">
+        <v>473</v>
+      </c>
+      <c r="C75" t="n">
+        <v>485</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
         <v>75</v>
       </c>
+      <c r="B76" t="n">
+        <v>343</v>
+      </c>
+      <c r="C76" t="n">
+        <v>243</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
         <v>76</v>
       </c>
+      <c r="B77" t="n">
+        <v>347</v>
+      </c>
+      <c r="C77" t="n">
+        <v>444</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
         <v>77</v>
       </c>
+      <c r="B78" t="n">
+        <v>359</v>
+      </c>
+      <c r="C78" t="n">
+        <v>192</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
         <v>78</v>
       </c>
+      <c r="B79" t="n">
+        <v>382</v>
+      </c>
+      <c r="C79" t="n">
+        <v>237</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
         <v>79</v>
       </c>
+      <c r="B80" t="n">
+        <v>499</v>
+      </c>
+      <c r="C80" t="n">
+        <v>68</v>
+      </c>
+      <c r="D80" t="n">
+        <v>197</v>
+      </c>
+      <c r="E80" t="n">
+        <v>322</v>
+      </c>
+      <c r="F80" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
         <v>80</v>
       </c>
+      <c r="B81" t="n">
+        <v>433</v>
+      </c>
+      <c r="C81" t="n">
+        <v>353</v>
+      </c>
+      <c r="D81" t="n">
+        <v>380</v>
+      </c>
+      <c r="E81" t="n">
+        <v>269</v>
+      </c>
+      <c r="F81" t="n">
+        <v>199</v>
+      </c>
+      <c r="G81" t="n">
+        <v>247</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
         <v>81</v>
       </c>
+      <c r="B82" t="n">
+        <v>389</v>
+      </c>
+      <c r="C82" t="n">
+        <v>421</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
         <v>82</v>
       </c>
+      <c r="B83" t="n">
+        <v>292</v>
+      </c>
+      <c r="C83" t="n">
+        <v>437</v>
+      </c>
+      <c r="D83" t="n">
+        <v>198</v>
+      </c>
+      <c r="E83" t="n">
+        <v>149</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
         <v>83</v>
       </c>
+      <c r="B84" t="n">
+        <v>154</v>
+      </c>
+      <c r="C84" t="n">
+        <v>462</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
         <v>84</v>
       </c>
+      <c r="B85" t="n">
+        <v>36</v>
+      </c>
+      <c r="C85" t="n">
+        <v>278</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
         <v>85</v>
       </c>
+      <c r="B86" t="n">
+        <v>115</v>
+      </c>
+      <c r="C86" t="n">
+        <v>383</v>
+      </c>
+      <c r="D86" t="n">
+        <v>431</v>
+      </c>
+      <c r="E86" t="n">
+        <v>159</v>
+      </c>
+      <c r="F86" t="n">
+        <v>387</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
         <v>86</v>
       </c>
+      <c r="B87" t="n">
+        <v>50</v>
+      </c>
+      <c r="C87" t="n">
+        <v>187</v>
+      </c>
+      <c r="D87" t="n">
+        <v>453</v>
+      </c>
+      <c r="E87" t="n">
+        <v>445</v>
+      </c>
+      <c r="F87" t="n">
+        <v>174</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
         <v>87</v>
       </c>
+      <c r="B88" t="n">
+        <v>331</v>
+      </c>
+      <c r="C88" t="n">
+        <v>418</v>
+      </c>
+      <c r="D88" t="n">
+        <v>205</v>
+      </c>
+      <c r="E88" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
         <v>88</v>
       </c>
+      <c r="B89" t="n">
+        <v>367</v>
+      </c>
+      <c r="C89" t="n">
+        <v>246</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
         <v>89</v>
       </c>
+      <c r="B90" t="n">
+        <v>18</v>
+      </c>
+      <c r="C90" t="n">
+        <v>38</v>
+      </c>
+      <c r="D90" t="n">
+        <v>242</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
         <v>90</v>
       </c>
+      <c r="B91" t="n">
+        <v>477</v>
+      </c>
+      <c r="C91" t="n">
+        <v>282</v>
+      </c>
+      <c r="D91" t="n">
+        <v>30</v>
+      </c>
+      <c r="E91" t="n">
+        <v>338</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
         <v>91</v>
       </c>
+      <c r="B92" t="n">
+        <v>91</v>
+      </c>
+      <c r="C92" t="n">
+        <v>42</v>
+      </c>
+      <c r="D92" t="n">
+        <v>226</v>
+      </c>
+      <c r="E92" t="n">
+        <v>176</v>
+      </c>
+      <c r="F92" t="n">
+        <v>79</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
         <v>92</v>
       </c>
+      <c r="B93" t="n">
+        <v>57</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
         <v>93</v>
       </c>
+      <c r="B94" t="n">
+        <v>155</v>
+      </c>
+      <c r="C94" t="n">
+        <v>25</v>
+      </c>
+      <c r="D94" t="n">
+        <v>312</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
         <v>94</v>
       </c>
+      <c r="B95" t="n">
+        <v>399</v>
+      </c>
+      <c r="C95" t="n">
+        <v>40</v>
+      </c>
+      <c r="D95" t="n">
+        <v>234</v>
+      </c>
+      <c r="E95" t="n">
+        <v>214</v>
+      </c>
+      <c r="F95" t="n">
+        <v>424</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
         <v>95</v>
       </c>
+      <c r="B96" t="n">
+        <v>466</v>
+      </c>
+      <c r="C96" t="n">
+        <v>309</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
         <v>96</v>
       </c>
+      <c r="B97" t="n">
+        <v>196</v>
+      </c>
+      <c r="C97" t="n">
+        <v>240</v>
+      </c>
+      <c r="D97" t="n">
+        <v>332</v>
+      </c>
+      <c r="E97" t="n">
+        <v>129</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
         <v>97</v>
+      </c>
+      <c r="B98" t="n">
+        <v>476</v>
+      </c>
+      <c r="C98" t="n">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="n">
+        <v>193</v>
+      </c>
+      <c r="C99" t="n">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" t="n">
+        <v>340</v>
+      </c>
+      <c r="C100" t="n">
+        <v>220</v>
+      </c>
+      <c r="D100" t="n">
+        <v>253</v>
+      </c>
+      <c r="E100" t="n">
+        <v>90</v>
+      </c>
+      <c r="F100" t="n">
+        <v>442</v>
+      </c>
+      <c r="G100" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" t="n">
+        <v>275</v>
+      </c>
+      <c r="C101" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" t="n">
+        <v>133</v>
+      </c>
+      <c r="C102" t="n">
+        <v>97</v>
+      </c>
+      <c r="D102" t="n">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" t="n">
+        <v>113</v>
+      </c>
+      <c r="C104" t="n">
+        <v>27</v>
+      </c>
+      <c r="D104" t="n">
+        <v>326</v>
+      </c>
+      <c r="E104" t="n">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" t="n">
+        <v>165</v>
+      </c>
+      <c r="C105" t="n">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" t="n">
+        <v>461</v>
+      </c>
+      <c r="C106" t="n">
+        <v>459</v>
+      </c>
+      <c r="D106" t="n">
+        <v>259</v>
+      </c>
+      <c r="E106" t="n">
+        <v>171</v>
+      </c>
+      <c r="F106" t="n">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>106</v>
+      </c>
+      <c r="B107" t="n">
+        <v>307</v>
+      </c>
+      <c r="C107" t="n">
+        <v>61</v>
+      </c>
+      <c r="D107" t="n">
+        <v>351</v>
+      </c>
+      <c r="E107" t="n">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>107</v>
+      </c>
+      <c r="B108" t="n">
+        <v>131</v>
+      </c>
+      <c r="C108" t="n">
+        <v>475</v>
+      </c>
+      <c r="D108" t="n">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>108</v>
+      </c>
+      <c r="B109" t="n">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>109</v>
+      </c>
+      <c r="B110" t="n">
+        <v>364</v>
+      </c>
+      <c r="C110" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>110</v>
+      </c>
+      <c r="B111" t="n">
+        <v>315</v>
+      </c>
+      <c r="C111" t="n">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>111</v>
+      </c>
+      <c r="B112" t="n">
+        <v>363</v>
+      </c>
+      <c r="C112" t="n">
+        <v>287</v>
+      </c>
+      <c r="D112" t="n">
+        <v>362</v>
+      </c>
+      <c r="E112" t="n">
+        <v>175</v>
+      </c>
+      <c r="F112" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" t="n">
+        <v>127</v>
+      </c>
+      <c r="C113" t="n">
+        <v>400</v>
+      </c>
+      <c r="D113" t="n">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" t="n">
+        <v>255</v>
+      </c>
+      <c r="C114" t="n">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>114</v>
+      </c>
+      <c r="B115" t="n">
+        <v>83</v>
+      </c>
+      <c r="C115" t="n">
+        <v>45</v>
+      </c>
+      <c r="D115" t="n">
+        <v>425</v>
+      </c>
+      <c r="E115" t="n">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>115</v>
+      </c>
+      <c r="B116" t="n">
+        <v>235</v>
+      </c>
+      <c r="C116" t="n">
+        <v>67</v>
+      </c>
+      <c r="D116" t="n">
+        <v>75</v>
+      </c>
+      <c r="E116" t="n">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>116</v>
+      </c>
+      <c r="B117" t="n">
+        <v>160</v>
+      </c>
+      <c r="C117" t="n">
+        <v>140</v>
+      </c>
+      <c r="D117" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>117</v>
+      </c>
+      <c r="B118" t="n">
+        <v>465</v>
+      </c>
+      <c r="C118" t="n">
+        <v>470</v>
+      </c>
+      <c r="D118" t="n">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>118</v>
+      </c>
+      <c r="B119" t="n">
+        <v>252</v>
+      </c>
+      <c r="C119" t="n">
+        <v>317</v>
+      </c>
+      <c r="D119" t="n">
+        <v>161</v>
+      </c>
+      <c r="E119" t="n">
+        <v>14</v>
+      </c>
+      <c r="F119" t="n">
+        <v>488</v>
+      </c>
+      <c r="G119" t="n">
+        <v>172</v>
+      </c>
+      <c r="H119" t="n">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>119</v>
+      </c>
+      <c r="B120" t="n">
+        <v>396</v>
+      </c>
+      <c r="C120" t="n">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>120</v>
+      </c>
+      <c r="B121" t="n">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>121</v>
+      </c>
+      <c r="B122" t="n">
+        <v>401</v>
+      </c>
+      <c r="C122" t="n">
+        <v>19</v>
+      </c>
+      <c r="D122" t="n">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>122</v>
+      </c>
+      <c r="B123" t="n">
+        <v>95</v>
+      </c>
+      <c r="C123" t="n">
+        <v>112</v>
+      </c>
+      <c r="D123" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>123</v>
+      </c>
+      <c r="B124" t="n">
+        <v>204</v>
+      </c>
+      <c r="C124" t="n">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>124</v>
+      </c>
+      <c r="B125" t="n">
+        <v>230</v>
+      </c>
+      <c r="C125" t="n">
+        <v>369</v>
+      </c>
+      <c r="D125" t="n">
+        <v>335</v>
+      </c>
+      <c r="E125" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>125</v>
+      </c>
+      <c r="B126" t="n">
+        <v>87</v>
+      </c>
+      <c r="C126" t="n">
+        <v>203</v>
+      </c>
+      <c r="D126" t="n">
+        <v>267</v>
+      </c>
+      <c r="E126" t="n">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>126</v>
+      </c>
+      <c r="B127" t="n">
+        <v>345</v>
+      </c>
+      <c r="C127" t="n">
+        <v>374</v>
+      </c>
+      <c r="D127" t="n">
+        <v>349</v>
+      </c>
+      <c r="E127" t="n">
+        <v>407</v>
+      </c>
+      <c r="F127" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>127</v>
+      </c>
+      <c r="B128" t="n">
+        <v>5</v>
+      </c>
+      <c r="C128" t="n">
+        <v>291</v>
+      </c>
+      <c r="D128" t="n">
+        <v>277</v>
+      </c>
+      <c r="E128" t="n">
+        <v>372</v>
+      </c>
+      <c r="F128" t="n">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>128</v>
+      </c>
+      <c r="B129" t="n">
+        <v>31</v>
+      </c>
+      <c r="C129" t="n">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>129</v>
+      </c>
+      <c r="B130" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>130</v>
+      </c>
+      <c r="B131" t="n">
+        <v>102</v>
+      </c>
+      <c r="C131" t="n">
+        <v>32</v>
+      </c>
+      <c r="D131" t="n">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>131</v>
+      </c>
+      <c r="B132" t="n">
+        <v>494</v>
+      </c>
+      <c r="C132" t="n">
+        <v>303</v>
+      </c>
+      <c r="D132" t="n">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>132</v>
+      </c>
+      <c r="B133" t="n">
+        <v>116</v>
+      </c>
+      <c r="C133" t="n">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>133</v>
+      </c>
+      <c r="B134" t="n">
+        <v>300</v>
+      </c>
+      <c r="C134" t="n">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>134</v>
+      </c>
+      <c r="B135" t="n">
+        <v>138</v>
+      </c>
+      <c r="C135" t="n">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>135</v>
+      </c>
+      <c r="B136" t="n">
+        <v>163</v>
+      </c>
+      <c r="C136" t="n">
+        <v>231</v>
+      </c>
+      <c r="D136" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>136</v>
+      </c>
+      <c r="B137" t="n">
+        <v>429</v>
+      </c>
+      <c r="C137" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>137</v>
+      </c>
+      <c r="B138" t="n">
+        <v>34</v>
+      </c>
+      <c r="C138" t="n">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>138</v>
+      </c>
+      <c r="B139" t="n">
+        <v>379</v>
+      </c>
+      <c r="C139" t="n">
+        <v>120</v>
+      </c>
+      <c r="D139" t="n">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>139</v>
+      </c>
+      <c r="B140" t="n">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>140</v>
+      </c>
+      <c r="B141" t="n">
+        <v>7</v>
+      </c>
+      <c r="C141" t="n">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>141</v>
+      </c>
+      <c r="B142" t="n">
+        <v>268</v>
+      </c>
+      <c r="C142" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>142</v>
+      </c>
+      <c r="B143" t="n">
+        <v>28</v>
+      </c>
+      <c r="C143" t="n">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>143</v>
+      </c>
+      <c r="B144" t="n">
+        <v>73</v>
+      </c>
+      <c r="C144" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>144</v>
+      </c>
+      <c r="B145" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>145</v>
+      </c>
+      <c r="B146" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>146</v>
+      </c>
+      <c r="B147" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>147</v>
+      </c>
+      <c r="B148" t="n">
+        <v>52</v>
+      </c>
+      <c r="C148" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" t="n">
+        <v>251</v>
+      </c>
+      <c r="C149" t="n">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>149</v>
+      </c>
+      <c r="B150" t="n">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>150</v>
+      </c>
+      <c r="B151" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" t="n">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" t="n">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>153</v>
+      </c>
+      <c r="B154" t="n">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="n">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="n">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="n">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="n">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="n">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="n">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="n">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="n">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="n">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="n">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="n">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="n">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="n">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="n">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="n">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="n">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="n">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="n">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="n">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="n">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="n">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="n">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="n">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="n">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="n">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="n">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="n">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="n">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="n">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="n">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="n">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="n">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="n">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="n">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="n">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="n">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="n">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="n">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="n">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="n">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="n">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="n">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="n">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="n">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="n">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="n">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="n">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="n">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="n">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="n">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="n">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="n">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="n">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="n">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="n">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="n">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="n">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="n">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="n">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="n">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="n">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="n">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="n">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="n">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="n">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="n">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="n">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="n">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="n">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="n">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="n">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="n">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="n">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="n">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="n">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="n">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="n">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="n">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="n">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="n">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="n">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="n">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="n">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="n">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="n">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="n">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="n">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="n">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="n">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="n">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="n">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="n">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="n">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="n">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="n">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="n">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="n">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="n">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="n">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="n">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="n">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="n">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="n">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="n">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="n">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="n">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="n">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="n">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="n">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="n">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="n">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="n">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="n">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="n">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="n">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="n">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="n">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="n">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="n">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="n">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="n">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="n">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="n">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="n">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="n">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="n">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="n">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="n">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="n">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="n">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="n">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="n">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="n">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="n">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="n">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="n">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="n">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="n">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="n">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="n">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="n">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="n">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="n">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="n">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="n">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="n">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="n">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="n">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="n">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="n">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="n">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="n">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="n">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="n">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="n">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="n">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>